<commit_message>
Uploading new work on Bankruptcies
</commit_message>
<xml_diff>
--- a/Resources/Political Control State-Level DF-Extract 2020-April.xlsx
+++ b/Resources/Political Control State-Level DF-Extract 2020-April.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23328"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brook\project-1-challenge\Resources\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{908625CF-D97C-4BE7-92CD-C3B913C5E7D8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="24240" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -277,8 +271,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -288,13 +282,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -334,34 +321,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -408,7 +381,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -440,27 +413,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -492,24 +447,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -685,41 +622,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:W51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="S34" sqref="S34"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.21875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.21875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.77734375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.21875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="12" style="3" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="12.88671875" style="3" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="13.88671875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="11" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="31.6640625" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:23">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -765,10 +675,10 @@
       <c r="P1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="Q1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="R1" s="1" t="s">
         <v>16</v>
       </c>
       <c r="S1" s="1" t="s">
@@ -787,7 +697,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:23">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -836,11 +746,11 @@
       <c r="P2" t="s">
         <v>72</v>
       </c>
-      <c r="Q2" s="3">
-        <v>0.22857142857142859</v>
-      </c>
-      <c r="R2" s="3">
-        <v>0.26666666666666672</v>
+      <c r="Q2">
+        <v>0.2285714285714286</v>
+      </c>
+      <c r="R2">
+        <v>0.2666666666666667</v>
       </c>
       <c r="S2" t="s">
         <v>75</v>
@@ -858,7 +768,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:23">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -907,10 +817,10 @@
       <c r="P3" t="s">
         <v>72</v>
       </c>
-      <c r="Q3" s="3">
+      <c r="Q3">
         <v>0.35</v>
       </c>
-      <c r="R3" s="3">
+      <c r="R3">
         <v>0.375</v>
       </c>
       <c r="S3" t="s">
@@ -929,7 +839,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:23">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -978,11 +888,11 @@
       <c r="P4" t="s">
         <v>72</v>
       </c>
-      <c r="Q4" s="3">
-        <v>0.43333333333333329</v>
-      </c>
-      <c r="R4" s="3">
-        <v>0.48333333333333328</v>
+      <c r="Q4">
+        <v>0.4333333333333333</v>
+      </c>
+      <c r="R4">
+        <v>0.4833333333333333</v>
       </c>
       <c r="S4" t="s">
         <v>76</v>
@@ -1000,7 +910,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:23">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -1049,10 +959,10 @@
       <c r="P5" t="s">
         <v>72</v>
       </c>
-      <c r="Q5" s="3">
-        <v>0.25714285714285712</v>
-      </c>
-      <c r="R5" s="3">
+      <c r="Q5">
+        <v>0.2571428571428571</v>
+      </c>
+      <c r="R5">
         <v>0.24</v>
       </c>
       <c r="S5" t="s">
@@ -1071,7 +981,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:23">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -1120,11 +1030,11 @@
       <c r="P6" t="s">
         <v>73</v>
       </c>
-      <c r="Q6" s="3">
-        <v>0.72499999999999998</v>
-      </c>
-      <c r="R6" s="3">
-        <v>0.76249999999999996</v>
+      <c r="Q6">
+        <v>0.725</v>
+      </c>
+      <c r="R6">
+        <v>0.7625</v>
       </c>
       <c r="S6" t="s">
         <v>77</v>
@@ -1142,7 +1052,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:23">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -1191,11 +1101,11 @@
       <c r="P7" t="s">
         <v>73</v>
       </c>
-      <c r="Q7" s="3">
-        <v>0.54285714285714282</v>
-      </c>
-      <c r="R7" s="3">
-        <v>0.63076923076923075</v>
+      <c r="Q7">
+        <v>0.5428571428571428</v>
+      </c>
+      <c r="R7">
+        <v>0.6307692307692307</v>
       </c>
       <c r="S7" t="s">
         <v>78</v>
@@ -1213,7 +1123,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:23">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -1262,11 +1172,11 @@
       <c r="P8" t="s">
         <v>73</v>
       </c>
-      <c r="Q8" s="3">
-        <v>0.61111111111111116</v>
-      </c>
-      <c r="R8" s="3">
-        <v>0.60264900662251653</v>
+      <c r="Q8">
+        <v>0.6111111111111112</v>
+      </c>
+      <c r="R8">
+        <v>0.6026490066225165</v>
       </c>
       <c r="S8" t="s">
         <v>77</v>
@@ -1284,7 +1194,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:23">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -1333,11 +1243,11 @@
       <c r="P9" t="s">
         <v>73</v>
       </c>
-      <c r="Q9" s="3">
+      <c r="Q9">
         <v>0.5714285714285714</v>
       </c>
-      <c r="R9" s="3">
-        <v>0.63414634146341464</v>
+      <c r="R9">
+        <v>0.6341463414634146</v>
       </c>
       <c r="S9" t="s">
         <v>78</v>
@@ -1355,7 +1265,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:23">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -1404,11 +1314,11 @@
       <c r="P10" t="s">
         <v>72</v>
       </c>
-      <c r="Q10" s="3">
-        <v>0.42499999999999999</v>
-      </c>
-      <c r="R10" s="3">
-        <v>0.39166666666666672</v>
+      <c r="Q10">
+        <v>0.425</v>
+      </c>
+      <c r="R10">
+        <v>0.3916666666666667</v>
       </c>
       <c r="S10" t="s">
         <v>76</v>
@@ -1426,7 +1336,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:23">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -1475,11 +1385,11 @@
       <c r="P11" t="s">
         <v>72</v>
       </c>
-      <c r="Q11" s="3">
+      <c r="Q11">
         <v>0.375</v>
       </c>
-      <c r="R11" s="3">
-        <v>0.41666666666666669</v>
+      <c r="R11">
+        <v>0.4166666666666667</v>
       </c>
       <c r="S11" t="s">
         <v>75</v>
@@ -1497,7 +1407,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:23">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -1546,11 +1456,11 @@
       <c r="P12" t="s">
         <v>73</v>
       </c>
-      <c r="Q12" s="3">
+      <c r="Q12">
         <v>0.96</v>
       </c>
-      <c r="R12" s="3">
-        <v>0.90196078431372551</v>
+      <c r="R12">
+        <v>0.9019607843137255</v>
       </c>
       <c r="S12" t="s">
         <v>77</v>
@@ -1568,7 +1478,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:23">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -1617,10 +1527,10 @@
       <c r="P13" t="s">
         <v>72</v>
       </c>
-      <c r="Q13" s="3">
+      <c r="Q13">
         <v>0.2</v>
       </c>
-      <c r="R13" s="3">
+      <c r="R13">
         <v>0.2</v>
       </c>
       <c r="S13" t="s">
@@ -1639,7 +1549,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:23">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -1688,10 +1598,10 @@
       <c r="P14" t="s">
         <v>73</v>
       </c>
-      <c r="Q14" s="3">
-        <v>0.67796610169491522</v>
-      </c>
-      <c r="R14" s="3">
+      <c r="Q14">
+        <v>0.6779661016949152</v>
+      </c>
+      <c r="R14">
         <v>0.6271186440677966</v>
       </c>
       <c r="S14" t="s">
@@ -1710,7 +1620,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:23">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -1759,10 +1669,10 @@
       <c r="P15" t="s">
         <v>72</v>
       </c>
-      <c r="Q15" s="3">
+      <c r="Q15">
         <v>0.2</v>
       </c>
-      <c r="R15" s="3">
+      <c r="R15">
         <v>0.33</v>
       </c>
       <c r="S15" t="s">
@@ -1781,7 +1691,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:23">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -1830,10 +1740,10 @@
       <c r="P16" t="s">
         <v>72</v>
       </c>
-      <c r="Q16" s="3">
+      <c r="Q16">
         <v>0.36</v>
       </c>
-      <c r="R16" s="3">
+      <c r="R16">
         <v>0.47</v>
       </c>
       <c r="S16" t="s">
@@ -1852,7 +1762,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:23">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -1901,11 +1811,11 @@
       <c r="P17" t="s">
         <v>74</v>
       </c>
-      <c r="Q17" s="3">
-        <v>0.27500000000000002</v>
-      </c>
-      <c r="R17" s="3">
-        <v>0.32800000000000001</v>
+      <c r="Q17">
+        <v>0.275</v>
+      </c>
+      <c r="R17">
+        <v>0.328</v>
       </c>
       <c r="S17" t="s">
         <v>75</v>
@@ -1923,7 +1833,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:23">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -1972,10 +1882,10 @@
       <c r="P18" t="s">
         <v>74</v>
       </c>
-      <c r="Q18" s="3">
-        <v>0.23684210526315791</v>
-      </c>
-      <c r="R18" s="3">
+      <c r="Q18">
+        <v>0.2368421052631579</v>
+      </c>
+      <c r="R18">
         <v>0.38</v>
       </c>
       <c r="S18" t="s">
@@ -1994,7 +1904,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:23">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -2043,11 +1953,11 @@
       <c r="P19" t="s">
         <v>74</v>
       </c>
-      <c r="Q19" s="3">
-        <v>0.30769230769230771</v>
-      </c>
-      <c r="R19" s="3">
-        <v>0.33333333333333331</v>
+      <c r="Q19">
+        <v>0.3076923076923077</v>
+      </c>
+      <c r="R19">
+        <v>0.3333333333333333</v>
       </c>
       <c r="S19" t="s">
         <v>75</v>
@@ -2065,7 +1975,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:23">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -2114,11 +2024,11 @@
       <c r="P20" t="s">
         <v>73</v>
       </c>
-      <c r="Q20" s="3">
+      <c r="Q20">
         <v>0.6</v>
       </c>
-      <c r="R20" s="3">
-        <v>0.58278145695364236</v>
+      <c r="R20">
+        <v>0.5827814569536424</v>
       </c>
       <c r="S20" t="s">
         <v>77</v>
@@ -2136,7 +2046,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:23">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -2185,11 +2095,11 @@
       <c r="P21" t="s">
         <v>74</v>
       </c>
-      <c r="Q21" s="3">
-        <v>0.68085106382978722</v>
-      </c>
-      <c r="R21" s="3">
-        <v>0.69503546099290781</v>
+      <c r="Q21">
+        <v>0.6808510638297872</v>
+      </c>
+      <c r="R21">
+        <v>0.6950354609929078</v>
       </c>
       <c r="S21" t="s">
         <v>77</v>
@@ -2207,7 +2117,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:23">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -2256,11 +2166,11 @@
       <c r="P22" t="s">
         <v>74</v>
       </c>
-      <c r="Q22" s="3">
+      <c r="Q22">
         <v>0.85</v>
       </c>
-      <c r="R22" s="3">
-        <v>0.78749999999999998</v>
+      <c r="R22">
+        <v>0.7875</v>
       </c>
       <c r="S22" t="s">
         <v>77</v>
@@ -2278,7 +2188,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:23">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -2327,11 +2237,11 @@
       <c r="P23" t="s">
         <v>74</v>
       </c>
-      <c r="Q23" s="3">
-        <v>0.42105263157894729</v>
-      </c>
-      <c r="R23" s="3">
-        <v>0.47272727272727272</v>
+      <c r="Q23">
+        <v>0.4210526315789473</v>
+      </c>
+      <c r="R23">
+        <v>0.4727272727272727</v>
       </c>
       <c r="S23" t="s">
         <v>76</v>
@@ -2349,7 +2259,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:23">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -2398,11 +2308,11 @@
       <c r="P24" t="s">
         <v>74</v>
       </c>
-      <c r="Q24" s="3">
-        <v>0.47761194029850751</v>
-      </c>
-      <c r="R24" s="3">
-        <v>0.55970149253731338</v>
+      <c r="Q24">
+        <v>0.4776119402985075</v>
+      </c>
+      <c r="R24">
+        <v>0.5597014925373134</v>
       </c>
       <c r="S24" t="s">
         <v>76</v>
@@ -2420,7 +2330,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:23">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -2469,11 +2379,11 @@
       <c r="P25" t="s">
         <v>72</v>
       </c>
-      <c r="Q25" s="3">
-        <v>0.30769230769230771</v>
-      </c>
-      <c r="R25" s="3">
-        <v>0.37704918032786883</v>
+      <c r="Q25">
+        <v>0.3076923076923077</v>
+      </c>
+      <c r="R25">
+        <v>0.3770491803278688</v>
       </c>
       <c r="S25" t="s">
         <v>75</v>
@@ -2491,7 +2401,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:23">
       <c r="A26" s="1">
         <v>24</v>
       </c>
@@ -2540,11 +2450,11 @@
       <c r="P26" t="s">
         <v>72</v>
       </c>
-      <c r="Q26" s="3">
-        <v>0.23529411764705879</v>
-      </c>
-      <c r="R26" s="3">
-        <v>0.29447852760736198</v>
+      <c r="Q26">
+        <v>0.2352941176470588</v>
+      </c>
+      <c r="R26">
+        <v>0.294478527607362</v>
       </c>
       <c r="S26" t="s">
         <v>75</v>
@@ -2562,7 +2472,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:23">
       <c r="A27" s="1">
         <v>25</v>
       </c>
@@ -2611,10 +2521,10 @@
       <c r="P27" t="s">
         <v>74</v>
       </c>
-      <c r="Q27" s="3">
+      <c r="Q27">
         <v>0.4</v>
       </c>
-      <c r="R27" s="3">
+      <c r="R27">
         <v>0.42</v>
       </c>
       <c r="S27" t="s">
@@ -2633,7 +2543,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:23">
       <c r="A28" s="1">
         <v>26</v>
       </c>
@@ -2682,7 +2592,7 @@
       <c r="P28">
         <v>0</v>
       </c>
-      <c r="Q28" s="3">
+      <c r="Q28">
         <v>0</v>
       </c>
       <c r="S28" t="s">
@@ -2701,7 +2611,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:23">
       <c r="A29" s="1">
         <v>27</v>
       </c>
@@ -2750,11 +2660,11 @@
       <c r="P29" t="s">
         <v>73</v>
       </c>
-      <c r="Q29" s="3">
-        <v>0.61904761904761907</v>
-      </c>
-      <c r="R29" s="3">
-        <v>0.66666666666666663</v>
+      <c r="Q29">
+        <v>0.6190476190476191</v>
+      </c>
+      <c r="R29">
+        <v>0.6666666666666666</v>
       </c>
       <c r="S29" t="s">
         <v>77</v>
@@ -2772,7 +2682,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="30" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:23">
       <c r="A30" s="1">
         <v>28</v>
       </c>
@@ -2821,11 +2731,11 @@
       <c r="P30" t="s">
         <v>74</v>
       </c>
-      <c r="Q30" s="3">
-        <v>0.58333333333333337</v>
-      </c>
-      <c r="R30" s="3">
-        <v>0.58499999999999996</v>
+      <c r="Q30">
+        <v>0.5833333333333334</v>
+      </c>
+      <c r="R30">
+        <v>0.585</v>
       </c>
       <c r="S30" t="s">
         <v>78</v>
@@ -2843,7 +2753,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="31" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:23">
       <c r="A31" s="1">
         <v>29</v>
       </c>
@@ -2892,10 +2802,10 @@
       <c r="P31" t="s">
         <v>73</v>
       </c>
-      <c r="Q31" s="3">
+      <c r="Q31">
         <v>0.625</v>
       </c>
-      <c r="R31" s="3">
+      <c r="R31">
         <v>0.65</v>
       </c>
       <c r="S31" t="s">
@@ -2914,7 +2824,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="32" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:23">
       <c r="A32" s="1">
         <v>30</v>
       </c>
@@ -2963,11 +2873,11 @@
       <c r="P32" t="s">
         <v>73</v>
       </c>
-      <c r="Q32" s="3">
-        <v>0.61904761904761907</v>
-      </c>
-      <c r="R32" s="3">
-        <v>0.65714285714285714</v>
+      <c r="Q32">
+        <v>0.6190476190476191</v>
+      </c>
+      <c r="R32">
+        <v>0.6571428571428571</v>
       </c>
       <c r="S32" t="s">
         <v>77</v>
@@ -2985,7 +2895,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="33" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:23">
       <c r="A33" s="1">
         <v>31</v>
       </c>
@@ -3034,11 +2944,11 @@
       <c r="P33" t="s">
         <v>73</v>
       </c>
-      <c r="Q33" s="3">
-        <v>0.63492063492063489</v>
-      </c>
-      <c r="R33" s="3">
-        <v>0.69333333333333336</v>
+      <c r="Q33">
+        <v>0.6349206349206349</v>
+      </c>
+      <c r="R33">
+        <v>0.6933333333333334</v>
       </c>
       <c r="S33" t="s">
         <v>77</v>
@@ -3056,7 +2966,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="34" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:23">
       <c r="A34" s="1">
         <v>32</v>
       </c>
@@ -3105,11 +3015,11 @@
       <c r="P34" t="s">
         <v>74</v>
       </c>
-      <c r="Q34" s="3">
+      <c r="Q34">
         <v>0.42</v>
       </c>
-      <c r="R34" s="3">
-        <v>0.45833333333333331</v>
+      <c r="R34">
+        <v>0.4583333333333333</v>
       </c>
       <c r="S34" t="s">
         <v>76</v>
@@ -3127,7 +3037,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="35" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:23">
       <c r="A35" s="1">
         <v>33</v>
       </c>
@@ -3176,11 +3086,11 @@
       <c r="P35" t="s">
         <v>72</v>
       </c>
-      <c r="Q35" s="3">
-        <v>0.21276595744680851</v>
-      </c>
-      <c r="R35" s="3">
-        <v>0.15957446808510639</v>
+      <c r="Q35">
+        <v>0.2127659574468085</v>
+      </c>
+      <c r="R35">
+        <v>0.1595744680851064</v>
       </c>
       <c r="S35" t="s">
         <v>75</v>
@@ -3198,7 +3108,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="36" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:23">
       <c r="A36" s="1">
         <v>34</v>
       </c>
@@ -3247,11 +3157,11 @@
       <c r="P36" t="s">
         <v>72</v>
       </c>
-      <c r="Q36" s="3">
-        <v>0.27272727272727271</v>
-      </c>
-      <c r="R36" s="3">
-        <v>0.38383838383838381</v>
+      <c r="Q36">
+        <v>0.2727272727272727</v>
+      </c>
+      <c r="R36">
+        <v>0.3838383838383838</v>
       </c>
       <c r="S36" t="s">
         <v>75</v>
@@ -3269,7 +3179,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="37" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:23">
       <c r="A37" s="1">
         <v>35</v>
       </c>
@@ -3318,10 +3228,10 @@
       <c r="P37" t="s">
         <v>72</v>
       </c>
-      <c r="Q37" s="3">
+      <c r="Q37">
         <v>0.1875</v>
       </c>
-      <c r="R37" s="3">
+      <c r="R37">
         <v>0.2277227722772277</v>
       </c>
       <c r="S37" t="s">
@@ -3340,7 +3250,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="38" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:23">
       <c r="A38" s="1">
         <v>36</v>
       </c>
@@ -3389,10 +3299,10 @@
       <c r="P38" t="s">
         <v>73</v>
       </c>
-      <c r="Q38" s="3">
+      <c r="Q38">
         <v>0.6</v>
       </c>
-      <c r="R38" s="3">
+      <c r="R38">
         <v>0.6166666666666667</v>
       </c>
       <c r="S38" t="s">
@@ -3411,7 +3321,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="39" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:23">
       <c r="A39" s="1">
         <v>37</v>
       </c>
@@ -3460,11 +3370,11 @@
       <c r="P39" t="s">
         <v>74</v>
       </c>
-      <c r="Q39" s="3">
+      <c r="Q39">
         <v>0.42</v>
       </c>
-      <c r="R39" s="3">
-        <v>0.45812807881773399</v>
+      <c r="R39">
+        <v>0.458128078817734</v>
       </c>
       <c r="S39" t="s">
         <v>76</v>
@@ -3482,7 +3392,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="40" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:23">
       <c r="A40" s="1">
         <v>38</v>
       </c>
@@ -3531,10 +3441,10 @@
       <c r="P40" t="s">
         <v>73</v>
       </c>
-      <c r="Q40" s="3">
-        <v>0.86842105263157898</v>
-      </c>
-      <c r="R40" s="3">
+      <c r="Q40">
+        <v>0.868421052631579</v>
+      </c>
+      <c r="R40">
         <v>0.88</v>
       </c>
       <c r="S40" t="s">
@@ -3553,7 +3463,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="41" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:23">
       <c r="A41" s="1">
         <v>39</v>
       </c>
@@ -3602,11 +3512,11 @@
       <c r="P41" t="s">
         <v>72</v>
       </c>
-      <c r="Q41" s="3">
-        <v>0.41304347826086962</v>
-      </c>
-      <c r="R41" s="3">
-        <v>0.35483870967741937</v>
+      <c r="Q41">
+        <v>0.4130434782608696</v>
+      </c>
+      <c r="R41">
+        <v>0.3548387096774194</v>
       </c>
       <c r="S41" t="s">
         <v>76</v>
@@ -3624,7 +3534,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="42" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:23">
       <c r="A42" s="1">
         <v>40</v>
       </c>
@@ -3673,11 +3583,11 @@
       <c r="P42" t="s">
         <v>72</v>
       </c>
-      <c r="Q42" s="3">
-        <v>0.14285714285714279</v>
-      </c>
-      <c r="R42" s="3">
-        <v>0.15714285714285711</v>
+      <c r="Q42">
+        <v>0.1428571428571428</v>
+      </c>
+      <c r="R42">
+        <v>0.1571428571428571</v>
       </c>
       <c r="S42" t="s">
         <v>75</v>
@@ -3695,7 +3605,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="43" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:23">
       <c r="A43" s="1">
         <v>41</v>
       </c>
@@ -3744,11 +3654,11 @@
       <c r="P43" t="s">
         <v>72</v>
       </c>
-      <c r="Q43" s="3">
-        <v>0.15151515151515149</v>
-      </c>
-      <c r="R43" s="3">
-        <v>0.26262626262626271</v>
+      <c r="Q43">
+        <v>0.1515151515151515</v>
+      </c>
+      <c r="R43">
+        <v>0.2626262626262627</v>
       </c>
       <c r="S43" t="s">
         <v>75</v>
@@ -3766,7 +3676,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="44" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:23">
       <c r="A44" s="1">
         <v>42</v>
       </c>
@@ -3815,10 +3725,10 @@
       <c r="P44" t="s">
         <v>72</v>
       </c>
-      <c r="Q44" s="3">
-        <v>0.38709677419354838</v>
-      </c>
-      <c r="R44" s="3">
+      <c r="Q44">
+        <v>0.3870967741935484</v>
+      </c>
+      <c r="R44">
         <v>0.44</v>
       </c>
       <c r="S44" t="s">
@@ -3837,7 +3747,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="45" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:23">
       <c r="A45" s="1">
         <v>43</v>
       </c>
@@ -3886,11 +3796,11 @@
       <c r="P45" t="s">
         <v>72</v>
       </c>
-      <c r="Q45" s="3">
+      <c r="Q45">
         <v>0.2068965517241379</v>
       </c>
-      <c r="R45" s="3">
-        <v>0.21333333333333329</v>
+      <c r="R45">
+        <v>0.2133333333333333</v>
       </c>
       <c r="S45" t="s">
         <v>75</v>
@@ -3908,7 +3818,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="46" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:23">
       <c r="A46" s="1">
         <v>44</v>
       </c>
@@ -3957,11 +3867,11 @@
       <c r="P46" t="s">
         <v>74</v>
       </c>
-      <c r="Q46" s="3">
-        <v>0.73333333333333328</v>
-      </c>
-      <c r="R46" s="3">
-        <v>0.62666666666666671</v>
+      <c r="Q46">
+        <v>0.7333333333333333</v>
+      </c>
+      <c r="R46">
+        <v>0.6266666666666667</v>
       </c>
       <c r="S46" t="s">
         <v>77</v>
@@ -3979,7 +3889,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="47" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:23">
       <c r="A47" s="1">
         <v>45</v>
       </c>
@@ -4028,11 +3938,11 @@
       <c r="P47" t="s">
         <v>73</v>
       </c>
-      <c r="Q47" s="3">
-        <v>0.52500000000000002</v>
-      </c>
-      <c r="R47" s="3">
-        <v>0.55000000000000004</v>
+      <c r="Q47">
+        <v>0.525</v>
+      </c>
+      <c r="R47">
+        <v>0.55</v>
       </c>
       <c r="S47" t="s">
         <v>78</v>
@@ -4050,7 +3960,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="48" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:23">
       <c r="A48" s="1">
         <v>46</v>
       </c>
@@ -4099,11 +4009,11 @@
       <c r="P48" t="s">
         <v>73</v>
       </c>
-      <c r="Q48" s="3">
-        <v>0.59183673469387754</v>
-      </c>
-      <c r="R48" s="3">
-        <v>0.58163265306122447</v>
+      <c r="Q48">
+        <v>0.5918367346938775</v>
+      </c>
+      <c r="R48">
+        <v>0.5816326530612245</v>
       </c>
       <c r="S48" t="s">
         <v>78</v>
@@ -4121,7 +4031,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="49" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:23">
       <c r="A49" s="1">
         <v>47</v>
       </c>
@@ -4170,10 +4080,10 @@
       <c r="P49" t="s">
         <v>72</v>
       </c>
-      <c r="Q49" s="3">
-        <v>0.41176470588235292</v>
-      </c>
-      <c r="R49" s="3">
+      <c r="Q49">
+        <v>0.4117647058823529</v>
+      </c>
+      <c r="R49">
         <v>0.41</v>
       </c>
       <c r="S49" t="s">
@@ -4192,7 +4102,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="50" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:23">
       <c r="A50" s="1">
         <v>48</v>
       </c>
@@ -4241,11 +4151,11 @@
       <c r="P50" t="s">
         <v>74</v>
       </c>
-      <c r="Q50" s="3">
-        <v>0.42424242424242431</v>
-      </c>
-      <c r="R50" s="3">
-        <v>0.36363636363636359</v>
+      <c r="Q50">
+        <v>0.4242424242424243</v>
+      </c>
+      <c r="R50">
+        <v>0.3636363636363636</v>
       </c>
       <c r="S50" t="s">
         <v>76</v>
@@ -4263,7 +4173,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="51" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:23">
       <c r="A51" s="1">
         <v>49</v>
       </c>
@@ -4312,10 +4222,10 @@
       <c r="P51" t="s">
         <v>72</v>
       </c>
-      <c r="Q51" s="3">
+      <c r="Q51">
         <v>0.1</v>
       </c>
-      <c r="R51" s="3">
+      <c r="R51">
         <v>0.15</v>
       </c>
       <c r="S51" t="s">

</xml_diff>